<commit_message>
Implemented journey time calculation
</commit_message>
<xml_diff>
--- a/2021-4121COMP-Team_Eclipse/Monday-Friday (Blackpool - Liverpool).xlsx
+++ b/2021-4121COMP-Team_Eclipse/Monday-Friday (Blackpool - Liverpool).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukaginley/Desktop/University/Software Engineering/Semester 2/Software Engineering Workshop (4121COMP)/Project Code/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt\git\2021-4121comp-team_eclipse\2021-4121COMP-Team_Eclipse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9BF584C0-72FB-F44C-A6C4-F422060EAD2F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D91546C3-185E-445F-A05C-81DEE6FB4AE2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15780" xr2:uid="{8F18EA43-9C1E-144B-8B14-979FA82976CA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8F18EA43-9C1E-144B-8B14-979FA82976CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,71 +42,63 @@
     <t>Poulton-le-Fylde</t>
   </si>
   <si>
-    <t xml:space="preserve">Kirkham &amp; Wesham </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Preston </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Leyland </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Euxton </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wigan North Western </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Byrn </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Garswood </t>
-  </si>
-  <si>
-    <t xml:space="preserve">St. Helens Central </t>
-  </si>
-  <si>
     <t>Thatto Heath</t>
   </si>
   <si>
-    <t xml:space="preserve">Eccleston Park </t>
+    <t>Liverpool Lime Street</t>
   </si>
   <si>
-    <t xml:space="preserve">Prescot </t>
+    <t>Edge Hill</t>
   </si>
   <si>
-    <t xml:space="preserve">Huyton </t>
+    <t>Wavertree Technology Park</t>
   </si>
   <si>
-    <t xml:space="preserve">Roby </t>
+    <t>Broad Green</t>
   </si>
   <si>
-    <t xml:space="preserve">Broad Green </t>
+    <t>Roby</t>
   </si>
   <si>
-    <t xml:space="preserve">Wavertree Technology Park </t>
+    <t>Huyton</t>
   </si>
   <si>
-    <t xml:space="preserve">Edge Hill </t>
+    <t>Prescot</t>
   </si>
   <si>
-    <t xml:space="preserve">Liverpool Lime Street </t>
+    <t>Eccleston Park</t>
+  </si>
+  <si>
+    <t>St Helens Central</t>
+  </si>
+  <si>
+    <t>Garswood</t>
+  </si>
+  <si>
+    <t>Bryn</t>
+  </si>
+  <si>
+    <t>Wigan North Western</t>
+  </si>
+  <si>
+    <t>Euxton Balshaw Lane</t>
+  </si>
+  <si>
+    <t>Leyland</t>
+  </si>
+  <si>
+    <t>Preston (Lancs)</t>
+  </si>
+  <si>
+    <t>Kirkham &amp; Wesham</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -134,9 +126,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,16 +445,16 @@
   <dimension ref="A1:AT19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" customWidth="1"/>
+    <col min="1" max="1" width="30.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="C1">
@@ -500,8 +491,8 @@
         <v>2159</v>
       </c>
     </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="C2">
@@ -538,9 +529,9 @@
         <v>2204</v>
       </c>
     </row>
-    <row r="3" spans="1:46" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
+    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>18</v>
       </c>
       <c r="C3">
         <v>617</v>
@@ -573,9 +564,9 @@
         <v>2116</v>
       </c>
     </row>
-    <row r="4" spans="1:46" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
+    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
       </c>
       <c r="C4">
         <v>629</v>
@@ -611,9 +602,9 @@
         <v>2224</v>
       </c>
     </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
+    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
       </c>
       <c r="C5">
         <v>634</v>
@@ -649,9 +640,9 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="6" spans="1:46" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
+    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>15</v>
       </c>
       <c r="C6">
         <v>638</v>
@@ -687,9 +678,9 @@
         <v>2233</v>
       </c>
     </row>
-    <row r="7" spans="1:46" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
+    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
       </c>
       <c r="B7">
         <v>621</v>
@@ -773,9 +764,9 @@
         <v>2242</v>
       </c>
     </row>
-    <row r="8" spans="1:46" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>7</v>
+    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
       </c>
       <c r="B8">
         <v>627</v>
@@ -829,9 +820,9 @@
         <v>2248</v>
       </c>
     </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>8</v>
+    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>12</v>
       </c>
       <c r="B9">
         <v>631</v>
@@ -888,9 +879,9 @@
         <v>2252</v>
       </c>
     </row>
-    <row r="10" spans="1:46" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>9</v>
+    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>11</v>
       </c>
       <c r="B10">
         <v>638</v>
@@ -977,9 +968,9 @@
         <v>2259</v>
       </c>
     </row>
-    <row r="11" spans="1:46" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>10</v>
+    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>2</v>
       </c>
       <c r="B11">
         <v>642</v>
@@ -1033,9 +1024,9 @@
         <v>2303</v>
       </c>
     </row>
-    <row r="12" spans="1:46" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>11</v>
+    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>10</v>
       </c>
       <c r="B12">
         <v>644</v>
@@ -1089,9 +1080,9 @@
         <v>2306</v>
       </c>
     </row>
-    <row r="13" spans="1:46" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>12</v>
+    <row r="13" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>9</v>
       </c>
       <c r="B13">
         <v>647</v>
@@ -1148,9 +1139,9 @@
         <v>2308</v>
       </c>
     </row>
-    <row r="14" spans="1:46" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>13</v>
+    <row r="14" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>8</v>
       </c>
       <c r="B14">
         <v>651</v>
@@ -1285,9 +1276,9 @@
         <v>2316</v>
       </c>
     </row>
-    <row r="15" spans="1:46" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>14</v>
+    <row r="15" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>7</v>
       </c>
       <c r="B15">
         <v>654</v>
@@ -1395,9 +1386,9 @@
         <v>2318</v>
       </c>
     </row>
-    <row r="16" spans="1:46" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>15</v>
+    <row r="16" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>6</v>
       </c>
       <c r="B16">
         <v>657</v>
@@ -1505,9 +1496,9 @@
         <v>2321</v>
       </c>
     </row>
-    <row r="17" spans="1:46" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>16</v>
+    <row r="17" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>5</v>
       </c>
       <c r="B17">
         <v>702</v>
@@ -1615,9 +1606,9 @@
         <v>2324</v>
       </c>
     </row>
-    <row r="18" spans="1:46" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>17</v>
+    <row r="18" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>4</v>
       </c>
       <c r="B18">
         <v>705</v>
@@ -1725,9 +1716,9 @@
         <v>2327</v>
       </c>
     </row>
-    <row r="19" spans="1:46" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>18</v>
+    <row r="19" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>3</v>
       </c>
       <c r="B19">
         <v>711</v>

</xml_diff>